<commit_message>
Rename book to story (#87)
</commit_message>
<xml_diff>
--- a/data/raw/AudioSegment.xlsx
+++ b/data/raw/AudioSegment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441A432F-87C7-3D47-8ED2-1E51228EDDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC67FD6-4457-A841-8832-113ED31F6DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="500" windowWidth="34560" windowHeight="21580" xr2:uid="{18A4F225-AC8C-C14A-A578-B1508D9DF6E2}"/>
+    <workbookView xWindow="8960" yWindow="620" windowWidth="34560" windowHeight="21580" xr2:uid="{18A4F225-AC8C-C14A-A578-B1508D9DF6E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,19 +194,19 @@
     <t>Relates To ID</t>
   </si>
   <si>
-    <t>BCH_001</t>
-  </si>
-  <si>
-    <t>BCH_002</t>
-  </si>
-  <si>
-    <t>BCH_003</t>
-  </si>
-  <si>
     <t>Authorship Resource</t>
   </si>
   <si>
     <t>Daniela Subotic, Noémi Villars-Amberg</t>
+  </si>
+  <si>
+    <t>SCH_001</t>
+  </si>
+  <si>
+    <t>SCH_002</t>
+  </si>
+  <si>
+    <t>SCH_003</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K11"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,7 +639,7 @@
         <v>51</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -700,10 +700,10 @@
         <v>21</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -732,7 +732,7 @@
         <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -764,7 +764,7 @@
         <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -793,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -825,10 +825,10 @@
         <v>41</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
         <v>53</v>
-      </c>
-      <c r="K7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -886,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -918,10 +918,10 @@
         <v>41</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -950,7 +950,7 @@
         <v>22</v>
       </c>
       <c r="K11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>